<commit_message>
Update script for the first quest and add initialization the user's flags from the script table Template.xlsx
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="193">
   <si>
     <t>id</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Rep_change</t>
-  </si>
-  <si>
-    <t>{"1":{"rep_pol":-1}}</t>
   </si>
   <si>
     <t>{self.player['Name']}, I need you in the office right now</t>
@@ -203,18 +200,419 @@
  -Why didn't you pick up the phone, you freak?</t>
   </si>
   <si>
-    <t>-Okay, let's get down to the deal.
-HERE IS THE END OF THE TEST FRAGMENT</t>
-  </si>
-  <si>
     <t>I am sleeping</t>
+  </si>
+  <si>
+    <t>-Okay, let's get down to the deal.</t>
+  </si>
+  <si>
+    <t>-Yeah</t>
+  </si>
+  <si>
+    <t>-The owner of the shop’s technical accessories was cruelly killed in his home. There is a strange symbol on his body - a lined corporative emblem.</t>
+  </si>
+  <si>
+    <t>-What corporation?</t>
+  </si>
+  <si>
+    <t>-And that's why this deal should be solved by the Blade Runner?</t>
+  </si>
+  <si>
+    <t>-Yes. You should solve this deal as soon as possible because this company is putting pressure on me. I think you understand, what will be with all of us, if you don't solve it.</t>
+  </si>
+  <si>
+    <t>-Actually, we are not in the jurisdiction of corporations</t>
+  </si>
+  <si>
+    <t>-Do you really believe in it? I thought you gave up your illusions in the process of working in our office.</t>
+  </si>
+  <si>
+    <t>-Have never believed, but it is sad.</t>
+  </si>
+  <si>
+    <t>-I believed that we should make people's lives safer</t>
+  </si>
+  <si>
+    <t>-Completely.</t>
+  </si>
+  <si>
+    <t>{"0":{"rep_pol":1}}</t>
+  </si>
+  <si>
+    <t>{"1":{"rep_pol":1}}</t>
+  </si>
+  <si>
+    <t>-An idealist. It's amazing how long you survive with us with such views. However, we need to work now.</t>
+  </si>
+  <si>
+    <t>-Okey.</t>
+  </si>
+  <si>
+    <t>{"0":{"night_flag":1},"1":{"rep_pol":-1}}</t>
+  </si>
+  <si>
+    <t>-I think you should start either from his house, where the killing was made or from his shop. I think this shop may be the real goal of the killers.</t>
+  </si>
+  <si>
+    <t>Go to the victim's home</t>
+  </si>
+  <si>
+    <t>Go to the victim's shop</t>
+  </si>
+  <si>
+    <t>-What will you do on my place?</t>
+  </si>
+  <si>
+    <t>night_flag == 1 25 26</t>
+  </si>
+  <si>
+    <t>-Probably, it's better to go to his shop. You reacted quickly to my call, you may have time to catch the criminal there.</t>
+  </si>
+  <si>
+    <t>-It's too late to try to catch somebody in his shop. And this is only because you didn't pick up the phone. Therefore, go to his home.</t>
+  </si>
+  <si>
+    <t>Finally you manage to catch her. You've already seen this symbol on a flyer in a bar where you drank last week. It threatened to destroy stores and destroy all sellers personally. Is the criminals' next target really a store?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While you are driving to the crime scene, a thought is obsessively beating in your brain through the pain of a hangover. </t>
+  </si>
+  <si>
+    <t>Try to catch it</t>
+  </si>
+  <si>
+    <t>Surrender to a hangover and sleep a bit</t>
+  </si>
+  <si>
+    <t>Turn back and go to the shop</t>
+  </si>
+  <si>
+    <t>Get to the crime scene</t>
+  </si>
+  <si>
+    <t>night_flag == 1 27 30</t>
+  </si>
+  <si>
+    <t>Press the gas pedal.</t>
+  </si>
+  <si>
+    <t>Drive accurately.</t>
+  </si>
+  <si>
+    <t>You arrive at the house where the victim lived. The first thing that catches your eye is the area where he lived. It is truly strange that an average merchant lived in such a poor area. What had brought him here, into such a wilderness?</t>
+  </si>
+  <si>
+    <t>Get out of the car</t>
+  </si>
+  <si>
+    <t>View everything from the window</t>
+  </si>
+  <si>
+    <t>Looking around the environment, at first nothing terrible is visible. A typical poor area of a large metropolis in the middle of the 21st century. Garbage around, shabby walls of houses with dirty curses on them. At any time of the day, there are a lot of strange personalities in such areas. If you look closely, you see several people who look like drug addicts. It seems that some kind of conflict is brewing.</t>
+  </si>
+  <si>
+    <t>Take out the gun and approach them</t>
+  </si>
+  <si>
+    <t>Approach them without a gun</t>
+  </si>
+  <si>
+    <t>Step into the building</t>
+  </si>
+  <si>
+    <t>Start in chase</t>
+  </si>
+  <si>
+    <t>Let them go</t>
+  </si>
+  <si>
+    <t>You catch up with one of the addicts. While running, you managed to pull out the gun.</t>
+  </si>
+  <si>
+    <t>- Stop, otherwise I'll shoot you!</t>
+  </si>
+  <si>
+    <t>-I just want to talk to you</t>
+  </si>
+  <si>
+    <t>With a dirty curse and a raised middle finger, the addict dived into some corner, and you realize that he disappeared.</t>
+  </si>
+  <si>
+    <t>Return to the building.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-I saw him earlier, it's a Blade Rnner! Run! </t>
+  </si>
+  <si>
+    <t>He turns around. In his eyes you see the fear of a cornered animal. In a desperate leap, he tries to get you. Instinctively, you shoot a gun and realize that you have just killed him. They were almost certainly replicants, especially since one of them recognized you. However, why they gathered near the merchant's house remains a mystery.</t>
+  </si>
+  <si>
+    <t>{"0":{"humanity":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"humanity":-2}}</t>
+  </si>
+  <si>
+    <t>{"1":{"humanity":1}}</t>
+  </si>
+  <si>
+    <t>-What are you doing here?</t>
+  </si>
+  <si>
+    <t>-You are right. I am here to find a murderer of the merchant, who lived here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems that despite the assumed bravado, drug addicts are very afraid of your gun. \n - We are here to get, mmm, some medicine. Usually here is an automaited point where we can get, mmm, medicines. </t>
+  </si>
+  <si>
+    <t>-Where is this point?</t>
+  </si>
+  <si>
+    <t>Junks part and you see a strange device that looks like a vending machine for drinks with a hole for money and a window for goods. Tube from it goes up and disappears somewhere inside the house. \n -It doesn't work for a whole day, and we don't know why.</t>
+  </si>
+  <si>
+    <t>-Okay, you are free. Now get out of here. I don't think that it will ever work again.</t>
+  </si>
+  <si>
+    <t>-We don't know anything about it. \n You see fear in their eyes and understand that they really don't know anything.</t>
+  </si>
+  <si>
+    <t>Go to the kitchen</t>
+  </si>
+  <si>
+    <t>Go to the bedroom</t>
+  </si>
+  <si>
+    <t>Here you discover some strange accessories. In them you identified devices for cooking synthetic drugs. That's the answer to why the merchant lived in a poor neighborhood. It seems he had business on the side. And he sold the goods through a tube running from the wall to a strange device from below. It's ironic how no one in power is interested in these areas, that even such a direct drug trade has not been stopped by anyone.</t>
+  </si>
+  <si>
+    <t>Return to the hall</t>
+  </si>
+  <si>
+    <t>Go to the store room</t>
+  </si>
+  <si>
+    <t>-"New era.inc". This corporation is closely connected to the replicant’s trade. Representatives of the company reported the death. They had to have some kind of deal with him, and when they arrived, they saw what they saw.</t>
+  </si>
+  <si>
+    <t>When you enter the apartment, you see the body with a symbol on it's chest. At first glance, there is nothing new here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to the table </t>
+  </si>
+  <si>
+    <t>Go to the safe</t>
+  </si>
+  <si>
+    <t>You find a crumpled letter. In it you find threats and demands to close the store and stop cooperating with the corporation. It seems that the only thing the senders have no complaints about is the creation of drugs. The letter is not signed, but it also has a crossed-out corporation symbol drawn on it.</t>
+  </si>
+  <si>
+    <t>It seems that here is something interesting. You find a safe under the bed.</t>
+  </si>
+  <si>
+    <t>You find several chemical schemes. You don't know much about chemistry, but it seems that this shop owner and part-time drug dealer was developing a special drug for replicants. Such that it causes the strongest addiction, but does not affect their performance, tying them to the owner (or corporation) even stronger, at the biochemical level.</t>
+  </si>
+  <si>
+    <t>{"0":{"let_flag": 1},"1":{"drug_flag": 1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"let_flag": 1}</t>
+  </si>
+  <si>
+    <t>{"0":{"drug_flag": 1}}</t>
+  </si>
+  <si>
+    <t>View the recordings from the camera in the hallway</t>
+  </si>
+  <si>
+    <t>View the recordings from the camera behind the front door</t>
+  </si>
+  <si>
+    <t>Here you discover the camera control system. It seems that the owner hung the camera in the hallway and behind the front door.</t>
+  </si>
+  <si>
+    <t>It seems someone has destroyed these records</t>
+  </si>
+  <si>
+    <t>Inspect the room</t>
+  </si>
+  <si>
+    <t>Almost by accident, you stumble upon another hiding place. It seems that the apartment had a system filming the face of everyone coming inside.</t>
+  </si>
+  <si>
+    <t>Scrutinize photos</t>
+  </si>
+  <si>
+    <t>You find your face, face of the young girl, faces of the two strange guys (on the one photo) and faces of the two representatives of the corporation (also on one photo)</t>
+  </si>
+  <si>
+    <t>While you are driving to the shop, you remember that you've already seen this symbol on a flyer in a bar where you drank last week. It threatened to destroy stores and destroy all sellers personally. Is the criminals' next target really a store?</t>
+  </si>
+  <si>
+    <t>{"0":{"photo_flag": 1}</t>
+  </si>
+  <si>
+    <t>Go back to the car</t>
+  </si>
+  <si>
+    <t>shop_flag &gt;= 1 50 51</t>
+  </si>
+  <si>
+    <t>It seems like you can close the deal</t>
+  </si>
+  <si>
+    <t>Go to the police office</t>
+  </si>
+  <si>
+    <t>It seems now it's worth going to the shop</t>
+  </si>
+  <si>
+    <t>Drug addicts look at you angrily, but seeing a gun they do not risk attacking. You hear the voice of one of them. \n -Who you are and what do you need from us? \n Another guy steps out of the crowd. \n -I saw him earlier, it's a Blade Runner!</t>
+  </si>
+  <si>
+    <t>Even at night, the shopping district in this city is full of life. It is here, under the cover of darkness, that information dealers, sneaky experts in the field of document forgery and other interesting personalities appear. But today you are not interested in them at all. You are heading to a small building, on the ground floor of which there is a shop of the murdered man.</t>
+  </si>
+  <si>
+    <t>Go into the shop</t>
+  </si>
+  <si>
+    <t>Look around</t>
+  </si>
+  <si>
+    <t>Drive to the shop</t>
+  </si>
+  <si>
+    <t>The door wouldn't budge, but fortunately you managed to crack the lock on it. You showed your police ID to several visitors of the shopping district who came up. No one wanted to argue with you, but now dozens of curious eyes are looking at you. You're in the store.</t>
+  </si>
+  <si>
+    <t>Inspect the cash register</t>
+  </si>
+  <si>
+    <t>Inspect warehouses</t>
+  </si>
+  <si>
+    <t>Inspect the goods</t>
+  </si>
+  <si>
+    <t>As soon as you want to take a closer look, a sharp smell of incendiary mixture hits you in the nose.</t>
+  </si>
+  <si>
+    <t>Go for the smell</t>
+  </si>
+  <si>
+    <t>Run out into the street</t>
+  </si>
+  <si>
+    <t>You enter the warehouse and see a hunched figure spilling incendiary mixture everywhere and about to set it on fire. A light flashes in her hand, and then the whole warehouse is illuminated by the flame of fire. The figure runs to the back entrance.</t>
+  </si>
+  <si>
+    <t>Run after the figure</t>
+  </si>
+  <si>
+    <t>You notice a nook with some waste. It seems there should be a back entrance.</t>
+  </si>
+  <si>
+    <t>Inspect the back entrance</t>
+  </si>
+  <si>
+    <t>The lock is broken. It seems someone went inside without the owner's notification. You seem to hear a noise inside.</t>
+  </si>
+  <si>
+    <t>Lurk in ambush</t>
+  </si>
+  <si>
+    <t>You attack a figure running out of the back entrance. After a short fight, you manage to detain her. Here you hear shouts: "Fire". It seems that the person you caught turned out to be an arsonist.</t>
+  </si>
+  <si>
+    <t>You notice a figure squeezing through people.</t>
+  </si>
+  <si>
+    <t>-Hold the arsonist!</t>
+  </si>
+  <si>
+    <t>It seems that in the crowd of panicked people, you missed the arsonist.</t>
+  </si>
+  <si>
+    <t>Wait for the firefighters to arrive</t>
+  </si>
+  <si>
+    <t>Give chase</t>
+  </si>
+  <si>
+    <t>With great difficulty you manage to catch the arsonist</t>
+  </si>
+  <si>
+    <t>{"1":{"ars_flag":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"ars_flag":1}}</t>
+  </si>
+  <si>
+    <t>-Who the hell are you?</t>
+  </si>
+  <si>
+    <t>-Your undoing, a servant of the corporation \n With these words, the arsonist clenched his teeth with force and swallowed. His eyes rolled back and he went limp.</t>
+  </si>
+  <si>
+    <t>Call the police and give them the body</t>
+  </si>
+  <si>
+    <t>While you are waiting for the firefighters to end their work, a little boy approaches you. He is dressed very poorly, it seems he is from the local street kids. \n -Mr., are you from police?</t>
+  </si>
+  <si>
+    <t>-I am Blade Runner</t>
+  </si>
+  <si>
+    <t>-Do you know if there was a girl in the house during the fire?</t>
+  </si>
+  <si>
+    <t>-Nobody except arsonist</t>
+  </si>
+  <si>
+    <t>-I hope she's alive</t>
+  </si>
+  <si>
+    <t>-Who is she?</t>
+  </si>
+  <si>
+    <t>-Didn't see anybody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-However, I see that you were nere the shop. Have you seen the girl? </t>
+  </si>
+  <si>
+    <t>She works in this shop, the maid of its owner. She is good, gave me some food. The merchant mocked her, but everyone still thought that she was bad. Only because she's a replicant.</t>
+  </si>
+  <si>
+    <t>-Do you know where did she live?</t>
+  </si>
+  <si>
+    <t>-What could she be doing in the store at night?</t>
+  </si>
+  <si>
+    <t>-The merchant often forced her to work at night, to clean the store. She wasn't in her closet and I thought she might be in the store.</t>
+  </si>
+  <si>
+    <t>-And where is her closet?</t>
+  </si>
+  <si>
+    <t>-In the next dorm. The owner wanted her to live next to the store and rented a room for her there. But as i said, she is not there.</t>
+  </si>
+  <si>
+    <t>-Lets take a look on it</t>
+  </si>
+  <si>
+    <t>night_flag == 1 52 70</t>
+  </si>
+  <si>
+    <t>In the morning, the shopping area seems a little sleepy. Of course, the main trade takes place here at night. Contrary to your fears, it seems that no one attacked the store at night.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,13 +627,26 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -250,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -260,6 +671,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -540,10 +954,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,7 +1056,7 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -650,28 +1064,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5">
         <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="195">
@@ -679,10 +1093,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2">
         <v>16</v>
@@ -693,10 +1107,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
       <c r="E7" s="2">
         <v>16</v>
@@ -707,10 +1121,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2">
         <v>16</v>
@@ -721,16 +1135,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G9">
         <v>13</v>
@@ -741,22 +1155,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10">
         <v>10</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10">
         <v>10</v>
@@ -767,10 +1181,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E11">
         <v>11</v>
@@ -781,10 +1195,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E12">
         <v>12</v>
@@ -795,10 +1209,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
         <v>39</v>
-      </c>
-      <c r="D13" t="s">
-        <v>40</v>
       </c>
       <c r="E13">
         <v>13</v>
@@ -809,22 +1223,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14">
         <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14">
         <v>14</v>
       </c>
       <c r="L14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -832,22 +1246,22 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15">
         <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15">
         <v>15</v>
       </c>
       <c r="L15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -855,64 +1269,1070 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16">
         <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L16" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="L16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="150">
+    <row r="18" spans="1:12" ht="60">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>7</v>
+      <c r="D18" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19">
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="2">
+        <v>22</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="2">
+        <v>23</v>
+      </c>
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="2">
+        <v>29</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="2">
+        <v>22</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="2">
+        <v>24</v>
+      </c>
+      <c r="L24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="2">
+        <v>22</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="2">
+        <v>27</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="2">
+        <v>27</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="2">
+        <v>28</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G28" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="7">
+        <v>29</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="2">
+        <v>40</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="2">
+        <v>32</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" s="2">
+        <v>33</v>
+      </c>
+      <c r="H32" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="2">
+        <v>37</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D34" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34">
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34">
+        <v>40</v>
+      </c>
+      <c r="L34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35">
+        <v>35</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35">
+        <v>36</v>
+      </c>
+      <c r="L35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" t="s">
+        <v>103</v>
+      </c>
+      <c r="E36">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="D37" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37">
+        <v>40</v>
+      </c>
+      <c r="L37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E40" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="D41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="2">
+        <v>41</v>
+      </c>
+      <c r="F41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41">
+        <v>42</v>
+      </c>
+      <c r="H41" t="s">
+        <v>120</v>
+      </c>
+      <c r="I41">
+        <v>45</v>
+      </c>
+      <c r="J41" t="s">
+        <v>141</v>
+      </c>
+      <c r="K41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="D42" t="s">
+        <v>119</v>
+      </c>
+      <c r="E42" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="2">
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43">
+        <v>44</v>
+      </c>
+      <c r="H43" t="s">
+        <v>119</v>
+      </c>
+      <c r="I43">
+        <v>40</v>
+      </c>
+      <c r="L43" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" s="2">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44">
+        <v>40</v>
+      </c>
+      <c r="L44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" t="s">
+        <v>123</v>
+      </c>
+      <c r="E45" s="2">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45">
+        <v>40</v>
+      </c>
+      <c r="L45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="2">
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46">
+        <v>47</v>
+      </c>
+      <c r="H46" t="s">
+        <v>119</v>
+      </c>
+      <c r="I46">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>134</v>
+      </c>
+      <c r="D47" t="s">
+        <v>132</v>
+      </c>
+      <c r="E47">
+        <v>47</v>
+      </c>
+      <c r="F47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47">
+        <v>48</v>
+      </c>
+      <c r="H47" t="s">
+        <v>119</v>
+      </c>
+      <c r="I47">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D48" t="s">
+        <v>131</v>
+      </c>
+      <c r="E48" s="2">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>135</v>
+      </c>
+      <c r="G48">
+        <v>48</v>
+      </c>
+      <c r="H48" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="2">
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>138</v>
+      </c>
+      <c r="D50" t="s">
+        <v>119</v>
+      </c>
+      <c r="E50" s="2">
+        <v>40</v>
+      </c>
+      <c r="L50" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" t="s">
+        <v>144</v>
+      </c>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" t="s">
+        <v>150</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="2">
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>149</v>
+      </c>
+      <c r="G53" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="D54" t="s">
+        <v>152</v>
+      </c>
+      <c r="E54" s="2">
+        <v>54</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54">
+        <v>54</v>
+      </c>
+      <c r="H54" t="s">
+        <v>154</v>
+      </c>
+      <c r="I54">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" t="s">
+        <v>156</v>
+      </c>
+      <c r="E55" s="2">
+        <v>55</v>
+      </c>
+      <c r="F55" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" t="s">
+        <v>159</v>
+      </c>
+      <c r="E56" s="2">
+        <v>56</v>
+      </c>
+      <c r="F56" t="s">
+        <v>157</v>
+      </c>
+      <c r="G56">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>160</v>
+      </c>
+      <c r="D57" t="s">
+        <v>161</v>
+      </c>
+      <c r="E57" s="2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>162</v>
+      </c>
+      <c r="D58" t="s">
+        <v>163</v>
+      </c>
+      <c r="E58" s="2">
+        <v>58</v>
+      </c>
+      <c r="L58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E60">
+        <v>60</v>
+      </c>
+      <c r="F60" t="s">
+        <v>169</v>
+      </c>
+      <c r="G60">
+        <v>61</v>
+      </c>
+      <c r="L60" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>167</v>
+      </c>
+      <c r="D61" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D63" t="s">
+        <v>175</v>
+      </c>
+      <c r="E63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>176</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E64">
+        <v>64</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64">
+        <v>64</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I64">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65">
+        <v>67</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G65">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E66">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E67">
+        <v>68</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G67">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E68">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E69">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E70">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>192</v>
+      </c>
+      <c r="D71" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="2">
+        <v>53</v>
+      </c>
+      <c r="F71" t="s">
+        <v>149</v>
+      </c>
+      <c r="G71" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more scripts and change the system of flags. Now new features can be add from the table without any error.
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirillsafonov/PycharmProjects/blade_runner_bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3512C82-9C1F-9048-851E-879C26C2E56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50DABA0-3663-4B43-AF33-098523534BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19300" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="449">
   <si>
     <t>id</t>
   </si>
@@ -411,15 +411,6 @@
     <t>You find several chemical schemes. You don't know much about chemistry, but it seems that this shop owner and part-time drug dealer was developing a special drug for replicants. Such that it causes the strongest addiction, but does not affect their performance, tying them to the owner (or corporation) even stronger, at the biochemical level.</t>
   </si>
   <si>
-    <t>{"0":{"let_flag": 1},"1":{"drug_flag": 1}}</t>
-  </si>
-  <si>
-    <t>{"0":{"let_flag": 1}</t>
-  </si>
-  <si>
-    <t>{"0":{"drug_flag": 1}}</t>
-  </si>
-  <si>
     <t>View the recordings from the camera in the hallway</t>
   </si>
   <si>
@@ -768,7 +759,622 @@
     <t>The group of replicants decided to destroy the seller, who was actually developing a powerful drug for the corporation. It causes the strongest addiction, but does not affect their performance, tying them to the owner (or corporation) even stronger, at the biochemical level. The maid was chosen as a weapon to commit the murder. She only needed a little push, because the merchant was raping and mocking her. After committing the crime, the girl left for her destination. Two of the group went to the merchant's apartment and tried to cover their tracks, as well as steal documents. They succeeded only partially, they did not find a safe with chemical circuits. Then they carved the symbol of the group on the victim's chest and fled. Subsequently, one of the members of the group was sent to set fire to the store.</t>
   </si>
   <si>
-    <t>{"0":{"photo_flag": 1}}</t>
+    <t>{"0":{"end_1":1},"1":{"end_1":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"end_2":1},"1":{"end_2":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"end_3":1},"1":{"end_3":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"end_4":1},"1":{"end_4":1}}</t>
+  </si>
+  <si>
+    <t>Deal 2. Meet the organization</t>
+  </si>
+  <si>
+    <t>After your failure, you have been working in the archives for two months. It is difficult to imagine another occupation as boring as it is useless as it is your work now. Today it seems that you are facing another equally long and boring day.</t>
+  </si>
+  <si>
+    <t>Submit to fate and go to work.</t>
+  </si>
+  <si>
+    <t>Take your time and sleep for a couple more hours.</t>
+  </si>
+  <si>
+    <t>{"0":{"drug_flag":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"let_flag":1},"1":{"drug_flag":1}}</t>
+  </si>
+  <si>
+    <t>Start reading the electronic report</t>
+  </si>
+  <si>
+    <t>Drink a cup of tea</t>
+  </si>
+  <si>
+    <t>The boss's call interrupts you from your chosen occupation. You haven't talked to him since the previous deal, therefore it is interesting why he needed you.</t>
+  </si>
+  <si>
+    <t>Go to the chief's office</t>
+  </si>
+  <si>
+    <t>end_1 &gt;= 1 97 101</t>
+  </si>
+  <si>
+    <t>After the investigation was successfully completed, your business went uphill. You have become more often involved in investigations and entrusted with more dangerous missions. However, thoughts about the mysterious organization are still haunting you.</t>
+  </si>
+  <si>
+    <t>Drive to the work</t>
+  </si>
+  <si>
+    <t>Nevertheless, it seems that something interesting is planned today. Probably, blade runners got new information about the group of replicants. The chief called you and promised a new case.</t>
+  </si>
+  <si>
+    <t>-Morning, {self.player['Name']}. I've been waiting for you. I think I have a task that you might be interested in.</t>
+  </si>
+  <si>
+    <t>Morning. What a case?</t>
+  </si>
+  <si>
+    <t>Sleepy and angry, you arrive at work and go to your cubicle. "Why should I systematize electronic archives at all? As if there are no computer programs for this." In addition, you have heard rumors that your colleagues have obtained information about the replicant grouping. It only made your mood worse</t>
+  </si>
+  <si>
+    <t>It seems that nobody noticed your absence. You bitterly think that probably even if you don't come to work, everyone will not care. "Why should I systematize electronic archives at all? As if there are no computer programs for this." In addition, you have heard rumors that your colleagues have obtained information about the replicant grouping. It only made your mood worse</t>
+  </si>
+  <si>
+    <t>Morning. I heard several rumors…</t>
+  </si>
+  <si>
+    <t>Our colleagues caught one replicant. Without going into details, he killed his master's daughter, with whom he was in love. A strange story. Probably, he was a member of the  group that may have been involved in the murder as part of your past case.</t>
+  </si>
+  <si>
+    <t>I think this deal is connected to them. Our colleagues caught one replicant. Without going into details, he killed his master's daughter, with whom he was in love. A strange story. Probably, he was a member of the  group that may have been involved in the murder as part of your past case.</t>
+  </si>
+  <si>
+    <t>-And what dou want from to do?</t>
+  </si>
+  <si>
+    <t>-From this replicant we got information about terrorist attack. But we don't know the time and the place. I want you to integrate into the group as a police spy. You have to get this information.</t>
+  </si>
+  <si>
+    <t>-Are you mad?</t>
+  </si>
+  <si>
+    <t>-Why me?</t>
+  </si>
+  <si>
+    <t>end_1 &gt;= 1 108 109</t>
+  </si>
+  <si>
+    <t>-I will tell you truth. This is very dangerous task. Probably it is close to the suicide. So, I decide to choose somebody, who needs to restore the reputation and is willing to take a risk.</t>
+  </si>
+  <si>
+    <t>-First of all, you had a contact with this group in your previous deal. I think that it is better to send somebode with such experience. Secondly, we have quite a few available blade runners right now, so the choice is not wide.</t>
+  </si>
+  <si>
+    <t>-Am I able to refuse?</t>
+  </si>
+  <si>
+    <t>-I think it is impossible</t>
+  </si>
+  <si>
+    <t>-Okay, it seems I have no choice</t>
+  </si>
+  <si>
+    <t>-Okay, I will do it.</t>
+  </si>
+  <si>
+    <t>-You can always refuse. At the same time, you can start looking for a new job.</t>
+  </si>
+  <si>
+    <t>-Well. I'll look for myself in the field of private investigations.</t>
+  </si>
+  <si>
+    <t>-Perhaps everything suits me here</t>
+  </si>
+  <si>
+    <t>-Okay, so, you are fired.</t>
+  </si>
+  <si>
+    <t>-I knew you'd take this case. Talk to John, it seems that he has developed two options for how to introduce you into the group. I'm not sure, though, that you'll like them.</t>
+  </si>
+  <si>
+    <t>Talk with John</t>
+  </si>
+  <si>
+    <t>-Why wouldn't I like them?</t>
+  </si>
+  <si>
+    <t>-They include, mmm, a sort of extreme.</t>
+  </si>
+  <si>
+    <t>You find John in a nervous state. It seems he wants to share his plans with you.</t>
+  </si>
+  <si>
+    <t>-Boss said you have some plans which include me</t>
+  </si>
+  <si>
+    <t>-Firstly, tell me what we plan to do with my face. I think there are replicants who know me.</t>
+  </si>
+  <si>
+    <t>-Okay, tell me about hem</t>
+  </si>
+  <si>
+    <t>-Well, there are two options, either the usual disguise, beard there, mustache, classics in general. Or we will act like people of the middle of the 21st century. A small plastic surgery without any special consequences, and you are unlikely to be recognized.</t>
+  </si>
+  <si>
+    <t>-Perhaps I prefer the classics</t>
+  </si>
+  <si>
+    <t>-I'm used to my face, but what do I need it for if I get killed?</t>
+  </si>
+  <si>
+    <t>-Okay. Now about exactly how we're going to get you into the group. We know that they themselves go out to angry replicants who have nowhere to go. That means we need to, uh, sell you to them.</t>
+  </si>
+  <si>
+    <t>-We know that they themselves go out to angry replicants who have nowhere to go. That means we need to, uh, sell you to them.</t>
+  </si>
+  <si>
+    <t>-Sell?...</t>
+  </si>
+  <si>
+    <t>{"0":{"trust_points":1},"1":{"trust_points":3}}</t>
+  </si>
+  <si>
+    <t>-Yeah. This means they must beliebe, that you are angry enough and that you are replicant. Also, we should show you them. We khow two places, where can be their representatives. The first one is a bar "Secondary people", popular among replicants. The second one is underground surgery for replicants.</t>
+  </si>
+  <si>
+    <t>-Why haven't we closed them yet?</t>
+  </si>
+  <si>
+    <t>-And the choice of location depends on how I will be, uh, "sold"?</t>
+  </si>
+  <si>
+    <t>-It's better to know their adress then not. Such places will emerge even if we close their predecessors.</t>
+  </si>
+  <si>
+    <t>-Okay. And the choice of location depends on how I will be, uh, "sold"?</t>
+  </si>
+  <si>
+    <t>-Yes. In the first case, you will be beaten by a blade runner near the bar, in the second you will get injured in the process of fleeing from the police.</t>
+  </si>
+  <si>
+    <t>-Bar is better</t>
+  </si>
+  <si>
+    <t>-Another ideas?...</t>
+  </si>
+  <si>
+    <t>-No. I'm sorry, but you should really suffer from us. In other cases, we cannot guarantee the result.</t>
+  </si>
+  <si>
+    <t>-Okay, let's go to the surgery</t>
+  </si>
+  <si>
+    <t>You go to the "Secondary People" bar. As a partner, you were given a taciturn blade runner with a square jaw and powerful muscles. It's very sad that he's actually going to beat you up.</t>
+  </si>
+  <si>
+    <t>Step into the bar</t>
+  </si>
+  <si>
+    <t>After 15 minutes, your colleague also enters the bar. Without further ado, he comes up to you, takes you by the jacket and starts swearing loudly at the whole bar. \n -You, dirty replicant. F***ing freak. How dare you steal money from me? I am Blde Runner.</t>
+  </si>
+  <si>
+    <t>-F*** you</t>
+  </si>
+  <si>
+    <t>-Just don't hit too hard</t>
+  </si>
+  <si>
+    <t>Spit in his face</t>
+  </si>
+  <si>
+    <t>Continuing to swear, a colleague begins methodically hitting you in the face. You're not sure he doesn't enjoy it.</t>
+  </si>
+  <si>
+    <t>Give back</t>
+  </si>
+  <si>
+    <t>Silently endure</t>
+  </si>
+  <si>
+    <t>Having finished his beating, your colleague glares at the bar patrons, barely restraining themselves from attacking him. He glares at them, threatens them with a gun, and leaves the bar, not forgetting to call you a replicant again.</t>
+  </si>
+  <si>
+    <t>- What a freak</t>
+  </si>
+  <si>
+    <t>- It hurts</t>
+  </si>
+  <si>
+    <t>{"0":{"trust_points":1},"1":{"trust_points":0}}</t>
+  </si>
+  <si>
+    <t>{"0":{"trust_points":2},"1":{"trust_points":-1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"trust_points":1},"1":{"trust_points":-1},"2":{"trust_points":3}}</t>
+  </si>
+  <si>
+    <t>One of the bar patrons comes up to you and helps you up. \n - It seems you've really annoyed this policeman</t>
+  </si>
+  <si>
+    <t>-Do you care?</t>
+  </si>
+  <si>
+    <t>-You have a hatred for people like him. I have a, uh, business proposition for you. Let's go sit down and talk.</t>
+  </si>
+  <si>
+    <t>-Interesting</t>
+  </si>
+  <si>
+    <t>You go with your colleague to the poor area where this underground clinic is located. You really don't like what's going on, but it seems that there is nowhere to retreat.</t>
+  </si>
+  <si>
+    <t>-You're not going to shoot me, are you?</t>
+  </si>
+  <si>
+    <t>-And what should we do if I can't get away from you properly?</t>
+  </si>
+  <si>
+    <t>-We both have instructions. \n He was right. You got instructions. According to plan, the end-point of the chase should be clinic. In the middle of the way, you should be injured, and then the pursuer will fall behind.</t>
+  </si>
+  <si>
+    <t>-Okay, let's get started</t>
+  </si>
+  <si>
+    <t>You go on the run. After waiting a couple of minutes, your colleague starts after you. At first you run in silence. Then you hear shouts behind "Hold the replicant" and "Stop or I'll shoot"</t>
+  </si>
+  <si>
+    <t>Run towards the clinic</t>
+  </si>
+  <si>
+    <t>In the middle of the way you hear a shot. After a moment, the shoulder explodes with pain, it seems that the injury meant exactly what you didn't want to think about. Suddenly you hear a cry from your colleague, and the thud of the body hitting the ground.</t>
+  </si>
+  <si>
+    <t>Go back</t>
+  </si>
+  <si>
+    <t>Continue running</t>
+  </si>
+  <si>
+    <t>Someone grabs your good shoulder. \n - Follow me quickly. I finished him off, but it's better not to light up.</t>
+  </si>
+  <si>
+    <t>-Who are you?</t>
+  </si>
+  <si>
+    <t>-What the hell is going on?</t>
+  </si>
+  <si>
+    <t>-All questions later. Now we should go to the clinic.</t>
+  </si>
+  <si>
+    <t>Follow the stranger</t>
+  </si>
+  <si>
+    <t>A stranger is catching up with you. \n - Are you running? You're doing the right thing. I'll meet you at the clinic. \n With these words, the stranger dived into an alley.</t>
+  </si>
+  <si>
+    <t>Run to the clinic</t>
+  </si>
+  <si>
+    <t>When you get to the underground clinic, you get help. It seems that your new acquaintance is well known here and therefore you are not charged.</t>
+  </si>
+  <si>
+    <t>Wait for further developments</t>
+  </si>
+  <si>
+    <t>Try to talk to your colleague's killer</t>
+  </si>
+  <si>
+    <t>A stranger approaches you. \n -My name is Shahryār. I save you from this blade runner. I have a deal for you.</t>
+  </si>
+  <si>
+    <t>-Don't think that I can give you anything</t>
+  </si>
+  <si>
+    <t>-Listen you</t>
+  </si>
+  <si>
+    <t>During that, uh, blade runner incident, you showed yourself to be quite physically resilient. Our group, a group of replicants, is fighting against the corporation that controls everything here, including these hunters. I can't tell you more yet, but I would like to invite you to join us.</t>
+  </si>
+  <si>
+    <t>-Do you have any ultimate goal?</t>
+  </si>
+  <si>
+    <t>-What unites you?</t>
+  </si>
+  <si>
+    <t>-How many replicants are there in your group?</t>
+  </si>
+  <si>
+    <t>-You will find out the answers to your questions later. Unfortunately, nowadays trust is a very expensive thing. But if you join us, I think you can earn it. If you agree to my proposal, here is the address for you, come to it, you will be met by a representative of the group. \n With these words, stranger hangs your hand and leave you alone.</t>
+  </si>
+  <si>
+    <t>Follow the address</t>
+  </si>
+  <si>
+    <t>Take a break</t>
+  </si>
+  <si>
+    <t>After a while, you arrive at the address. It seems that now there is a long way to go to trust on the part of replicants.</t>
+  </si>
+  <si>
+    <t>One day, you were summoned by one of the group commanders to a small meeting.</t>
+  </si>
+  <si>
+    <t>Go to a meeting</t>
+  </si>
+  <si>
+    <t>{"0":{"injury":1},"1":{"injury":0}}</t>
+  </si>
+  <si>
+    <t>You're looking around the room you came to. Four replicants are sitting at a cramped table. Two more guards are standing at the door. There are several charts and lists on the table. It seems that the audience is discussing some important plans.</t>
+  </si>
+  <si>
+    <t>-Did you want to see me?</t>
+  </si>
+  <si>
+    <t>Yes. You see, we are moving to the final stage of the operation and it seems that it's time to get rid of unreliable elements.</t>
+  </si>
+  <si>
+    <t>-What do you mean?</t>
+  </si>
+  <si>
+    <t>-It seems you understand the truth</t>
+  </si>
+  <si>
+    <t>-Well, how else? \n The guards slowly began to move towards you. It seems you should run. But documents. They're so close.</t>
+  </si>
+  <si>
+    <t>Escape through the window</t>
+  </si>
+  <si>
+    <t>Abruptly push the guard away and run through the corridor</t>
+  </si>
+  <si>
+    <t>Try to grab the documents and run away</t>
+  </si>
+  <si>
+    <t>trust_points &gt;= 10 162 164</t>
+  </si>
+  <si>
+    <t>Your behavior has earned our trust. We offer you to participate in our final operation. In the one for which our group was created. We are going to completely destroy the workshops and the head office of the "New Era.inc".</t>
+  </si>
+  <si>
+    <t>-What needs to be done?</t>
+  </si>
+  <si>
+    <t>-Can I refuse?</t>
+  </si>
+  <si>
+    <t>Sure. However, in any case, this is the last operation of our group, so you will have to leave it. However, even if one of us survives the operation, it is unlikely that we will be able to continue our activities.</t>
+  </si>
+  <si>
+    <t>-Well, then goodbye</t>
+  </si>
+  <si>
+    <t>-I am in</t>
+  </si>
+  <si>
+    <t>Go to the police and prevent</t>
+  </si>
+  <si>
+    <t>Stay and fight on the replicant side</t>
+  </si>
+  <si>
+    <t>Walk away from the city</t>
+  </si>
+  <si>
+    <t>To the end</t>
+  </si>
+  <si>
+    <t>You participated in the replicant attack on the corporation. Like the other attackers, you died as a result of its commission. The performance of your group prompted other groups of replicants to protest, as well as those who supported them. It is unlikely that they will succeed, but there is always hope, isn't there?</t>
+  </si>
+  <si>
+    <t>injury &gt;= 1 171 172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An attack was prevented. All members of the group were caught and eliminated. The award was issued to you personally by the head of the corporation. {"On the director's desk you see a drug developed according to the schemes you found."*min(1, self.Player['drug_flag'])} </t>
+  </si>
+  <si>
+    <t>You lean over the table, and the leaders begin to explain their plan. You are amazed by the scale and number of replicants involved. Only in the evening you leave the building. You are shaking, because you understand that an attack is scheduled for tomorrow, and it seems that you have too little time left to make a final choice.</t>
+  </si>
+  <si>
+    <t>It seems you've really given up on this case. As a result of the attack, several thousand people were killed, including ordinary workers. Did you want this outcome?</t>
+  </si>
+  <si>
+    <t>-Oh, hi, {self.player['Name']}. I have two different plans, how we can integrate you into this rebel group.</t>
+  </si>
+  <si>
+    <t>You went to another city. Waking up two days later, you hear about the attacks in the news. To your surprise, you note that apparently not all of the planned attacks were successful and far fewer people were injured than planned.</t>
+  </si>
+  <si>
+    <t>You couldn't get any information. As a result, the whole operation failed and you were dismissed from the police. Waking up two days later, you hear about the attacks in the news.</t>
+  </si>
+  <si>
+    <t>A wounded shoulder that has not fully healed deprives you of your former agility.  The guards grab you and start strangling you. With the last effort you manage to escape and jump out through the window. You didn't pick up the documents. As a result, the whole operation failed and you were dismissed from the police. Waking up two days later, you hear about the attacks in the news.</t>
+  </si>
+  <si>
+    <t>You manage to grab the documents and escape from the guards, who did not expect you to be so quick. With difficulty breaking away from the chase, you stop to catch your breath.</t>
+  </si>
+  <si>
+    <t>Give in to a hunch</t>
+  </si>
+  <si>
+    <t>You take photos of several documents. Then you compose a letter to the head of the corporation, including in it the requirements for curtailing drug development and improving the living conditions of replicants. You also offer a time and place for negotiations with replicants. Then you compose a letter to the replicants. In it, you ask to curtail the preparation of attacks and offer a time and place for negotiations. You throw it under the door of one of the members of the group the same night. You are not sure that you will be able to reconcile everyone, but perhaps you will be able to bring everyone to the negotiating table...</t>
+  </si>
+  <si>
+    <t>We are glad to see that you complete our game. This game was developed by Kirill and Mikhail as a creativity project for our course "Fantastic in World Literatue". We are grateful to our teacher and peer-reviewers for their valuable help in our project. \n The story is inspired by the film "Blade Runner" (1982) by Ridley Scott and novel "Do Androids Dream of Electric Sheep?" by Philip K. Dick. \n The story was created as an element of fun-fiction culture onlu for non-commercial purposes. \n All characters appearing in this work are fictitious. Any resemblance to real persons, living or dead, or real events or actions is purely coincidental. \n References: \n Philip K. Dick (1968). "Do Androids Dream of Electric Sheep?". \n Ridley Scott (1982). "Blade runner".</t>
+  </si>
+  <si>
+    <t>Restart deal 1</t>
+  </si>
+  <si>
+    <t>Restart deal 2</t>
+  </si>
+  <si>
+    <t>Come to the woman.</t>
+  </si>
+  <si>
+    <t>Come to the man</t>
+  </si>
+  <si>
+    <t>Here you found a spacious room full of replicants of all kinds. Two replicants: a man and a woman are clearly interested in you.</t>
+  </si>
+  <si>
+    <t>Hi, {self.player['Name']}! My name is Roxy and I have a deal for you. It’s a chance to prove that you’re loyal to our organization. I want you to drive with me. I will tell you everything later.</t>
+  </si>
+  <si>
+    <t>Come to the man.</t>
+  </si>
+  <si>
+    <t>Well, you are again in that spacious room. The man is waiting for you.</t>
+  </si>
+  <si>
+    <t>Yeah, sure!</t>
+  </si>
+  <si>
+    <t>No, I’m not interested.</t>
+  </si>
+  <si>
+    <t>You got into Roxy’s car. She seems absolutely calm but suddenly her face contorted.</t>
+  </si>
+  <si>
+    <t>Ignore Roxy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - What happened?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - I just saw a restaurant of one fast food chain. I worked in one for two years and I don’t want to share this experience with you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - You can trust me. What happened there?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - No problem, let’s forget this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - The manager in the restaurant abused his power and made me work for 20 hours a day. He beat me up while no one sees and publicly humiliated me in front of clients. Once one client got mad at me because he thought that I wasn’t fast enough. The client slapped me and spat in my face. After that accident, the manager yelled at me for about an hour and told that I was utterly useless. He said that I had to clean up the freezer room and when I started, he locked me up inside it for the whole night. I nearly died that time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - How did you escape?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Let’s talk about something else.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - When he opened the door in the morning the next day, I stabbed him with a butcher knife and he died. After this revenge I run away. I wandered along the streets and lived in abandoned buildings. Finally, I found home and the purpose to live here. Humans were never kind to me. I hate them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - It seems that it was a very difficult time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - How did you dare to kill a human?</t>
+  </si>
+  <si>
+    <t>Return to the spacious room.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Let’s talk about our deal. A freight train full of the things we need will be passing by today. Our mission is to get on the train at the station where it makes a stop, get to the end of the train and uncouple the last few cars. Others will do the rest.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Get out of my car, freak!</t>
+  </si>
+  <si>
+    <t>Say, "Okey, I'm in."</t>
+  </si>
+  <si>
+    <t>Say, "I don't want to do anything illegal!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It was quite easy for us to sneak unnoticed on the train at the station. And everything was good until we uncoupled the cars. A security guard appeared out of nowhere and captured Roxy. I was on the uncoupled part of the train rapidly losing its speed while Roxy and the guard were on the main part of the train. </t>
+  </si>
+  <si>
+    <t>Jump and try to help Roxy.</t>
+  </si>
+  <si>
+    <t>Do nothing and take no risks.</t>
+  </si>
+  <si>
+    <t>You pushed the guard away and he almost fell off the train. Roxy, once free, wanted to finally throw off the guard.</t>
+  </si>
+  <si>
+    <t>Stop her.</t>
+  </si>
+  <si>
+    <t>Let her kill him.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If I don’t do it, he will kill us. I just have to. </t>
+  </si>
+  <si>
+    <t>Trust me! Nothing bad will happen.</t>
+  </si>
+  <si>
+    <t>Agree with her.</t>
+  </si>
+  <si>
+    <t>When the guard was able to get up, he took out a gun and aimed it at you. When he almost pulled the trigger, Roxy lunged at him. The bullet hit her and they both fell off the train. They both were dead.</t>
+  </si>
+  <si>
+    <t>There is a little time to reflect.</t>
+  </si>
+  <si>
+    <t>Think about how to escape from the train.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roxy knew me literally for a few hours. Why did she sacrifice her life to save me? I tried to gain their trust, but both the person and the replicant died because of me. I should have let her kill this man but I couldn’t. Was it worth it? </t>
+  </si>
+  <si>
+    <t>Do it!</t>
+  </si>
+  <si>
+    <t>There were a lot of buttons and levers in the control room, but you think you figured out how to stop it.</t>
+  </si>
+  <si>
+    <t>Stop the train.</t>
+  </si>
+  <si>
+    <t>Suddenly you noticed the group of 5 men working on the railway tracks. They saw you too late and have no chance to run away from the train. Surprisingly there is another track and you can turn the train this way. What will you do?</t>
+  </si>
+  <si>
+    <t>Do nothing and the train will kill these 5 men.</t>
+  </si>
+  <si>
+    <t>Turn the train and it will kill only one man.</t>
+  </si>
+  <si>
+    <t>You made your choice. 5 people were dead. Nevertheless, the train stopped and you escaped. You told all the story to other replicants.</t>
+  </si>
+  <si>
+    <t>You made your choice. Only one person was dead. But he was innocent. Nevertheless, the train stopped and you escaped. You told all the story to other replicants.</t>
+  </si>
+  <si>
+    <t>You made your choice. You told all the story to other replicants. Nobody knows where Roxy is now and if she is alive.</t>
+  </si>
+  <si>
+    <t>She did it. You can still hear him screaming! But Roxy doesn't worry at all. For her, it's a common thing to kill humans. She thanked you and said that you were right when you had allowed her to kill the guard. \n Roxy added, "If you go to Colt's café, you can find my safe there. The pin code is P451. You can take all the money from it. It's a gift from me."</t>
+  </si>
+  <si>
+    <t>Well… Thank you. Let's think about how to escape from the train.</t>
+  </si>
+  <si>
+    <t>You can get to the head of the train and try to stop it.</t>
+  </si>
+  <si>
+    <t>{"0":{"let_flag":1}}</t>
+  </si>
+  <si>
+    <t>{"0":{"photo_flag":1}}</t>
+  </si>
+  <si>
+    <t>The man patted me on the shoulder and said that he's an owner of one café in the neighborhood. His name was Colt and he asked me to help him.</t>
   </si>
 </sst>
 </file>
@@ -799,10 +1405,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -815,7 +1420,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +1437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -845,7 +1450,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1126,15 +1738,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="116" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -1194,17 +1807,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3">
+    <row r="3" spans="1:12" s="7" customFormat="1">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>3</v>
       </c>
     </row>
@@ -1492,10 +2105,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D19" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E19" s="2">
         <v>90</v>
@@ -1702,19 +2315,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D30" t="s">
         <v>87</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>88</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1768,7 +2381,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>108</v>
@@ -1928,10 +2541,10 @@
         <v>45</v>
       </c>
       <c r="J41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1974,7 +2587,7 @@
         <v>40</v>
       </c>
       <c r="L43" t="s">
-        <v>127</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -1997,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="L44" t="s">
-        <v>129</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -2020,7 +2633,7 @@
         <v>40</v>
       </c>
       <c r="L45" t="s">
-        <v>128</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2028,16 +2641,16 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E46" s="2">
         <v>46</v>
       </c>
       <c r="F46" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G46">
         <v>47</v>
@@ -2054,16 +2667,16 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E47">
         <v>47</v>
       </c>
       <c r="F47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G47">
         <v>48</v>
@@ -2080,16 +2693,16 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E48" s="2">
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G48">
         <v>48</v>
@@ -2106,10 +2719,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E49" s="2">
         <v>49</v>
@@ -2126,7 +2739,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D50" t="s">
         <v>118</v>
@@ -2135,7 +2748,7 @@
         <v>40</v>
       </c>
       <c r="L50" t="s">
-        <v>246</v>
+        <v>447</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -2143,16 +2756,16 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F51" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G51" s="2">
         <v>91</v>
@@ -2163,16 +2776,16 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L52" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -2180,16 +2793,16 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E53" s="2">
         <v>53</v>
       </c>
       <c r="F53" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G53" s="2">
         <v>56</v>
@@ -2200,22 +2813,22 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D54" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E54" s="2">
         <v>54</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G54">
         <v>54</v>
       </c>
       <c r="H54" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="I54">
         <v>54</v>
@@ -2226,16 +2839,16 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E55" s="2">
         <v>55</v>
       </c>
       <c r="F55" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G55">
         <v>56</v>
@@ -2246,16 +2859,16 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E56" s="2">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F56" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G56">
         <v>59</v>
@@ -2266,10 +2879,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D57" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E57" s="2">
         <v>57</v>
@@ -2280,16 +2893,16 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E58" s="2">
         <v>58</v>
       </c>
       <c r="L58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -2297,10 +2910,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E59" s="2">
         <v>62</v>
@@ -2311,22 +2924,22 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E60">
         <v>60</v>
       </c>
       <c r="F60" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G60">
         <v>61</v>
       </c>
       <c r="L60" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -2334,10 +2947,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E61" s="2">
         <v>63</v>
@@ -2348,10 +2961,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="E62">
         <v>62</v>
@@ -2362,10 +2975,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E63">
         <v>63</v>
@@ -2376,10 +2989,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E64">
         <v>64</v>
@@ -2402,16 +3015,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E65">
         <v>67</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G65">
         <v>66</v>
@@ -2422,10 +3035,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E66">
         <v>67</v>
@@ -2436,16 +3049,16 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E67">
         <v>68</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G67">
         <v>69</v>
@@ -2456,10 +3069,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E68">
         <v>66</v>
@@ -2470,10 +3083,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E69">
         <v>71</v>
@@ -2484,10 +3097,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E70">
         <v>68</v>
@@ -2498,16 +3111,16 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D71" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E71" s="2">
         <v>53</v>
       </c>
       <c r="F71" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G71" s="2">
         <v>56</v>
@@ -2518,10 +3131,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D72" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E72" s="2">
         <v>72</v>
@@ -2532,10 +3145,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D73" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E73" s="2">
         <v>73</v>
@@ -2546,10 +3159,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D74" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E74" s="2">
         <v>74</v>
@@ -2566,7 +3179,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D75" t="s">
         <v>95</v>
@@ -2580,16 +3193,16 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E76" s="2">
         <v>76</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G76" s="2">
         <v>83</v>
@@ -2600,16 +3213,16 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D77" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E77" s="2">
         <v>77</v>
       </c>
       <c r="F77" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G77">
         <v>77</v>
@@ -2620,22 +3233,22 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E78" s="2">
         <v>78</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G78">
         <v>81</v>
       </c>
       <c r="L78" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -2643,16 +3256,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E79" s="2">
         <v>79</v>
       </c>
       <c r="F79" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G79">
         <v>80</v>
@@ -2663,16 +3276,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E80" s="2">
         <v>82</v>
       </c>
       <c r="F80" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G80">
         <v>80</v>
@@ -2683,10 +3296,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E81" s="2">
         <v>81</v>
@@ -2697,28 +3310,28 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D82" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E82" s="2">
         <v>94</v>
       </c>
       <c r="F82" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H82" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="L82" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -2726,10 +3339,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D83" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E83" s="2">
         <v>80</v>
@@ -2740,10 +3353,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D84" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E84" s="2">
         <v>80</v>
@@ -2754,22 +3367,22 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E85" s="2">
         <v>85</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G85">
         <v>85</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I85">
         <v>85</v>
@@ -2780,22 +3393,22 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D86" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E86" s="2">
         <v>87</v>
       </c>
       <c r="F86" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G86">
         <v>86</v>
       </c>
       <c r="L86" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -2803,19 +3416,19 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D87" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E87" s="2">
         <v>94</v>
       </c>
       <c r="F87" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -2823,25 +3436,25 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D88" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E88" s="2">
         <v>94</v>
       </c>
       <c r="F88" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H88" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -2849,16 +3462,16 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D89" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F89" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G89" s="2">
         <v>91</v>
@@ -2869,21 +3482,22 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D90" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E90" s="2">
         <v>30</v>
       </c>
+      <c r="G90" s="2"/>
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="2">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D91" t="s">
         <v>7</v>
@@ -2891,90 +3505,1583 @@
       <c r="E91" s="2">
         <v>1</v>
       </c>
+      <c r="G91" s="2"/>
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="2">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D92" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E92" s="2">
         <v>95</v>
       </c>
       <c r="F92" t="s">
-        <v>238</v>
-      </c>
-      <c r="G92" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="G92" s="2">
+        <v>96</v>
+      </c>
+      <c r="L92" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="2">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D93" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E93">
         <v>95</v>
       </c>
       <c r="F93" t="s">
-        <v>238</v>
-      </c>
-      <c r="G93" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="G93" s="2">
+        <v>96</v>
+      </c>
+      <c r="L93" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="2">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="D94" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E94" s="2">
         <v>95</v>
       </c>
       <c r="F94" t="s">
-        <v>238</v>
-      </c>
-      <c r="G94" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="G94" s="2">
+        <v>96</v>
+      </c>
+      <c r="L94" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="2">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D95" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E95">
         <v>95</v>
       </c>
       <c r="F95" t="s">
-        <v>238</v>
-      </c>
-      <c r="G95" s="7"/>
+        <v>235</v>
+      </c>
+      <c r="G95" s="2">
+        <v>96</v>
+      </c>
+      <c r="L95" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="2">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D96" t="s">
-        <v>238</v>
-      </c>
-      <c r="E96" s="8"/>
+        <v>235</v>
+      </c>
+      <c r="E96" s="6">
+        <v>96</v>
+      </c>
+      <c r="G96" s="2"/>
+    </row>
+    <row r="97" spans="1:9" s="7" customFormat="1">
+      <c r="A97" s="7">
+        <v>96</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>248</v>
+      </c>
+      <c r="D98" t="s">
+        <v>249</v>
+      </c>
+      <c r="E98">
+        <v>98</v>
+      </c>
+      <c r="F98" t="s">
+        <v>250</v>
+      </c>
+      <c r="G98" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>263</v>
+      </c>
+      <c r="D99" t="s">
+        <v>253</v>
+      </c>
+      <c r="E99">
+        <v>100</v>
+      </c>
+      <c r="F99" t="s">
+        <v>254</v>
+      </c>
+      <c r="G99" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>264</v>
+      </c>
+      <c r="D100" t="s">
+        <v>253</v>
+      </c>
+      <c r="E100">
+        <v>100</v>
+      </c>
+      <c r="F100" t="s">
+        <v>254</v>
+      </c>
+      <c r="G100">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>255</v>
+      </c>
+      <c r="D101" t="s">
+        <v>256</v>
+      </c>
+      <c r="E101" s="2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>258</v>
+      </c>
+      <c r="D102" t="s">
+        <v>259</v>
+      </c>
+      <c r="E102">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>260</v>
+      </c>
+      <c r="D103" t="s">
+        <v>256</v>
+      </c>
+      <c r="E103">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="2">
+        <v>104</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D104" t="s">
+        <v>262</v>
+      </c>
+      <c r="E104">
+        <v>105</v>
+      </c>
+      <c r="F104" t="s">
+        <v>265</v>
+      </c>
+      <c r="G104">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="2">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>266</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E105">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="2">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>267</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E106">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="2">
+        <v>107</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E107" t="s">
+        <v>272</v>
+      </c>
+      <c r="F107" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G107">
+        <v>110</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I107">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="2">
+        <v>108</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E108">
+        <v>110</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G108">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" s="2">
+        <v>109</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="E109">
+        <v>110</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="G109">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" s="2">
+        <v>110</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E110">
+        <v>111</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="G110">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" s="2">
+        <v>111</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D111" t="s">
+        <v>2</v>
+      </c>
+      <c r="E111">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" s="2">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>385</v>
+      </c>
+      <c r="D112" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="A113" s="2">
+        <v>113</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D113" t="s">
+        <v>284</v>
+      </c>
+      <c r="E113">
+        <v>115</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G113">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="A114" s="2">
+        <v>114</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D114" t="s">
+        <v>284</v>
+      </c>
+      <c r="E114">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="A115" s="2">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>287</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E115">
+        <v>116</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G115">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12">
+      <c r="A116" s="2">
+        <v>116</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E116">
+        <v>117</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G116">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="A117" s="2">
+        <v>117</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E117">
+        <v>119</v>
+      </c>
+      <c r="F117" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="G117">
+        <v>119</v>
+      </c>
+      <c r="L117" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="2">
+        <v>118</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E118">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="A119" s="2">
+        <v>119</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="E119">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="A120" s="2">
+        <v>120</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E120">
+        <v>121</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G120">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="A121" s="2">
+        <v>121</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="E121">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12">
+      <c r="A122" s="2">
+        <v>122</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E122">
+        <v>124</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G122" s="2">
+        <v>130</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="I122">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="A123" s="2">
+        <v>123</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E123">
+        <v>124</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G123" s="2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="A124" s="2">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>308</v>
+      </c>
+      <c r="D124" t="s">
+        <v>309</v>
+      </c>
+      <c r="E124">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="A125" s="2">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>310</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E125">
+        <v>126</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G125">
+        <v>126</v>
+      </c>
+      <c r="H125" t="s">
+        <v>313</v>
+      </c>
+      <c r="I125">
+        <v>126</v>
+      </c>
+      <c r="L125" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12">
+      <c r="A126" s="2">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>314</v>
+      </c>
+      <c r="D126" t="s">
+        <v>315</v>
+      </c>
+      <c r="E126">
+        <v>127</v>
+      </c>
+      <c r="F126" t="s">
+        <v>316</v>
+      </c>
+      <c r="G126">
+        <v>127</v>
+      </c>
+      <c r="L126" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="A127" s="2">
+        <v>127</v>
+      </c>
+      <c r="B127" t="s">
+        <v>317</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E127">
+        <v>128</v>
+      </c>
+      <c r="F127" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="G127">
+        <v>128</v>
+      </c>
+      <c r="L127" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="A128" s="2">
+        <v>128</v>
+      </c>
+      <c r="B128" t="s">
+        <v>323</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E128">
+        <v>129</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="G128">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12">
+      <c r="A129" s="2">
+        <v>129</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E129" s="2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12">
+      <c r="A130" s="2">
+        <v>130</v>
+      </c>
+      <c r="B130" t="s">
+        <v>327</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E130">
+        <v>131</v>
+      </c>
+      <c r="F130" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G130">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12">
+      <c r="A131" s="2">
+        <v>131</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="E131">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12">
+      <c r="A132" s="2">
+        <v>132</v>
+      </c>
+      <c r="B132" t="s">
+        <v>332</v>
+      </c>
+      <c r="D132" t="s">
+        <v>333</v>
+      </c>
+      <c r="E132">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12">
+      <c r="A133" s="2">
+        <v>133</v>
+      </c>
+      <c r="B133" t="s">
+        <v>334</v>
+      </c>
+      <c r="D133" t="s">
+        <v>335</v>
+      </c>
+      <c r="E133">
+        <v>134</v>
+      </c>
+      <c r="F133" t="s">
+        <v>336</v>
+      </c>
+      <c r="G133" s="2">
+        <v>136</v>
+      </c>
+      <c r="L133" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12">
+      <c r="A134" s="2">
+        <v>134</v>
+      </c>
+      <c r="B134" t="s">
+        <v>337</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E134">
+        <v>135</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G134">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12">
+      <c r="A135" s="2">
+        <v>135</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D135" t="s">
+        <v>341</v>
+      </c>
+      <c r="E135">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12">
+      <c r="A136" s="2">
+        <v>136</v>
+      </c>
+      <c r="B136" t="s">
+        <v>342</v>
+      </c>
+      <c r="D136" t="s">
+        <v>343</v>
+      </c>
+      <c r="E136">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12">
+      <c r="A137" s="2">
+        <v>137</v>
+      </c>
+      <c r="B137" t="s">
+        <v>344</v>
+      </c>
+      <c r="D137" t="s">
+        <v>346</v>
+      </c>
+      <c r="E137">
+        <v>138</v>
+      </c>
+      <c r="F137" t="s">
+        <v>345</v>
+      </c>
+      <c r="G137">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12">
+      <c r="A138" s="2">
+        <v>138</v>
+      </c>
+      <c r="B138" t="s">
+        <v>347</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E138">
+        <v>139</v>
+      </c>
+      <c r="F138" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="G138">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12">
+      <c r="A139" s="2">
+        <v>139</v>
+      </c>
+      <c r="B139" t="s">
+        <v>350</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E139">
+        <v>140</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G139">
+        <v>140</v>
+      </c>
+      <c r="H139" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="I139">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12">
+      <c r="A140" s="2">
+        <v>140</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D140" t="s">
+        <v>355</v>
+      </c>
+      <c r="E140">
+        <v>141</v>
+      </c>
+      <c r="F140" t="s">
+        <v>356</v>
+      </c>
+      <c r="G140">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12">
+      <c r="A141" s="2">
+        <v>141</v>
+      </c>
+      <c r="B141" t="s">
+        <v>357</v>
+      </c>
+      <c r="D141" t="s">
+        <v>2</v>
+      </c>
+      <c r="E141">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" s="7" customFormat="1">
+      <c r="A142" s="7">
+        <v>142</v>
+      </c>
+      <c r="B142" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="D142" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="E142" s="7">
+        <v>143</v>
+      </c>
+      <c r="F142" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="G142" s="7">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12">
+      <c r="A143" s="2">
+        <v>143</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D143" t="s">
+        <v>402</v>
+      </c>
+      <c r="E143">
+        <v>145</v>
+      </c>
+      <c r="F143" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="G143">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12">
+      <c r="A144">
+        <v>144</v>
+      </c>
+      <c r="B144" t="s">
+        <v>401</v>
+      </c>
+      <c r="D144" t="s">
+        <v>400</v>
+      </c>
+      <c r="E144">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145">
+        <v>145</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>404</v>
+      </c>
+      <c r="D145" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="E145">
+        <v>146</v>
+      </c>
+      <c r="F145" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="G145">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146">
+        <v>146</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E146">
+        <v>147</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="G146">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147">
+        <v>147</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D147" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="E147">
+        <v>148</v>
+      </c>
+      <c r="F147" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="G147">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7">
+      <c r="A148">
+        <v>148</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="E148">
+        <v>150</v>
+      </c>
+      <c r="F148" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="G148">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7">
+      <c r="A149">
+        <v>149</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E149">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" s="2" customFormat="1">
+      <c r="A150" s="2">
+        <v>150</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="D150" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="E150" s="2">
+        <v>151</v>
+      </c>
+      <c r="F150" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="G150" s="2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="2">
+        <v>151</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="E151" s="2">
+        <v>152</v>
+      </c>
+      <c r="F151" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="G151" s="2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="2">
+        <v>152</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="D152" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E152" s="2">
+        <v>153</v>
+      </c>
+      <c r="F152" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="G152" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="2">
+        <v>153</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="D153" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="E153" s="2">
+        <v>154</v>
+      </c>
+      <c r="F153" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="G153" s="2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7">
+      <c r="A154" s="2">
+        <v>154</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E154" s="2">
+        <v>155</v>
+      </c>
+      <c r="F154" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="G154">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7">
+      <c r="A155" s="2">
+        <v>155</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="D155" t="s">
+        <v>432</v>
+      </c>
+      <c r="E155" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7">
+      <c r="A156" s="2">
+        <v>156</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>445</v>
+      </c>
+      <c r="D156" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E156" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7">
+      <c r="A157" s="2">
+        <v>157</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D157" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E157" s="2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7">
+      <c r="A158" s="2">
+        <v>158</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="D158" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="E158" s="2">
+        <v>200</v>
+      </c>
+      <c r="F158" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="G158">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="2">
+        <v>200</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E159" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="2">
+        <v>201</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>441</v>
+      </c>
+      <c r="D160" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E160" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="2">
+        <v>202</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="D161" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="E161" s="2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="2">
+        <v>203</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="E162" s="2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" s="2">
+        <v>204</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
+      <c r="A164">
+        <v>160</v>
+      </c>
+      <c r="B164" t="s">
+        <v>358</v>
+      </c>
+      <c r="D164" t="s">
+        <v>359</v>
+      </c>
+      <c r="E164">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
+      <c r="A165">
+        <v>161</v>
+      </c>
+      <c r="B165" t="s">
+        <v>361</v>
+      </c>
+      <c r="D165" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="E165" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
+      <c r="A166">
+        <v>162</v>
+      </c>
+      <c r="B166" t="s">
+        <v>363</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E166">
+        <v>163</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G166">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
+      <c r="A167">
+        <v>163</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E167" s="6">
+        <v>169</v>
+      </c>
+      <c r="F167" t="s">
+        <v>368</v>
+      </c>
+      <c r="G167" s="2">
+        <v>169</v>
+      </c>
+      <c r="H167" t="s">
+        <v>369</v>
+      </c>
+      <c r="I167" s="7" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
+      <c r="A168">
+        <v>164</v>
+      </c>
+      <c r="B168" t="s">
+        <v>371</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="E168">
+        <v>166</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="G168">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
+      <c r="A169">
+        <v>165</v>
+      </c>
+      <c r="B169" t="s">
+        <v>374</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="E169">
+        <v>166</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="G169" s="2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
+      <c r="A170">
+        <v>166</v>
+      </c>
+      <c r="B170" t="s">
+        <v>384</v>
+      </c>
+      <c r="D170" t="s">
+        <v>377</v>
+      </c>
+      <c r="E170" s="2">
+        <v>167</v>
+      </c>
+      <c r="F170" t="s">
+        <v>378</v>
+      </c>
+      <c r="G170" s="2">
+        <v>170</v>
+      </c>
+      <c r="H170" t="s">
+        <v>379</v>
+      </c>
+      <c r="I170" s="2">
+        <v>168</v>
+      </c>
+      <c r="J170" t="s">
+        <v>391</v>
+      </c>
+      <c r="K170">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
+      <c r="A171">
+        <v>167</v>
+      </c>
+      <c r="B171" t="s">
+        <v>383</v>
+      </c>
+      <c r="D171" t="s">
+        <v>380</v>
+      </c>
+      <c r="E171" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
+      <c r="A172">
+        <v>168</v>
+      </c>
+      <c r="B172" t="s">
+        <v>387</v>
+      </c>
+      <c r="D172" t="s">
+        <v>380</v>
+      </c>
+      <c r="E172" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="A173">
+        <v>169</v>
+      </c>
+      <c r="B173" t="s">
+        <v>388</v>
+      </c>
+      <c r="D173" t="s">
+        <v>380</v>
+      </c>
+      <c r="E173" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11">
+      <c r="A174">
+        <v>170</v>
+      </c>
+      <c r="B174" t="s">
+        <v>381</v>
+      </c>
+      <c r="D174" t="s">
+        <v>380</v>
+      </c>
+      <c r="E174" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="A175">
+        <v>171</v>
+      </c>
+      <c r="B175" t="s">
+        <v>389</v>
+      </c>
+      <c r="D175" t="s">
+        <v>380</v>
+      </c>
+      <c r="E175" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
+      <c r="A176">
+        <v>172</v>
+      </c>
+      <c r="B176" t="s">
+        <v>390</v>
+      </c>
+      <c r="D176" t="s">
+        <v>377</v>
+      </c>
+      <c r="E176">
+        <v>167</v>
+      </c>
+      <c r="F176" t="s">
+        <v>391</v>
+      </c>
+      <c r="G176">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7">
+      <c r="A177">
+        <v>173</v>
+      </c>
+      <c r="B177" t="s">
+        <v>392</v>
+      </c>
+      <c r="D177" t="s">
+        <v>380</v>
+      </c>
+      <c r="E177">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7">
+      <c r="A178">
+        <v>174</v>
+      </c>
+      <c r="B178" t="s">
+        <v>393</v>
+      </c>
+      <c r="D178" t="s">
+        <v>394</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178" t="s">
+        <v>395</v>
+      </c>
+      <c r="G178">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
It's a finished draft. It must work from the beginning to the end but there are likely many bugs
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirillsafonov/PycharmProjects/blade_runner_bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A17676D-96B3-3A46-9AD3-5D84D9B44739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA018EB9-5D51-5046-93B8-E04644942D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="485">
   <si>
     <t>id</t>
   </si>
@@ -1140,9 +1140,6 @@
     <t>Try to grab the documents and run away</t>
   </si>
   <si>
-    <t>trust_points &gt;= 10 162 164</t>
-  </si>
-  <si>
     <t>Your behavior has earned our trust. We offer you to participate in our final operation. In the one for which our group was created. We are going to completely destroy the workshops and the head office of the "New Era.inc".</t>
   </si>
   <si>
@@ -1377,9 +1374,6 @@
     <t>She asked, "Why do I have to trust you?" After this words, she threw the guard out of the train.\nShe did it. You can still hear him screaming! But Roxy doesn't worry at all. For her, it's a common thing to kill humans.</t>
   </si>
   <si>
-    <t>Well…Let's think about how to escape from the train.</t>
-  </si>
-  <si>
     <t>roxy == 1 154 205</t>
   </si>
   <si>
@@ -1389,17 +1383,113 @@
     <t>{"0":{"roxy":1},"1":{"trust_points":-1}}</t>
   </si>
   <si>
-    <t>{"1":{"humanity":-1}}</t>
-  </si>
-  <si>
-    <t>{"0":{"trust_points":2}}</t>
+    <t>{"0":{"trust_points":3}}</t>
+  </si>
+  <si>
+    <t>-Sure, I will help you!</t>
+  </si>
+  <si>
+    <t>-I'm not interested.</t>
+  </si>
+  <si>
+    <t>{"0":{"humanity":1},"1":{"humanity":-1}}</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Read the previous message again.</t>
+  </si>
+  <si>
+    <t>You came to the cafe and changed into work clothes. You found a safe locked by the pin code. Do you want to try to open it?</t>
+  </si>
+  <si>
+    <t>Well… Let's think about how to escape from the train.</t>
+  </si>
+  <si>
+    <t>{"0":{"key":1}}</t>
+  </si>
+  <si>
+    <t>key == 1 209 210</t>
+  </si>
+  <si>
+    <t>You remembered the password that Roxy gave you. You entered P451 code and unlocked the safe. You found here 200 coins! Well done!</t>
+  </si>
+  <si>
+    <t>You tried a few combinations but it didn't work.</t>
+  </si>
+  <si>
+    <t>You returned to work and the first customers came in. They were four people: men and women. They said that they lived on the same street and their houses were side by side in the same row. The first person lives in house number 1, the second person lives in house number 2 and so on. They gave you some tips to understand who prefers which kind of coffee.\n1. Women drink only latte.\n2. The Russian woman who live in the 4th house has a bird.\n3. The German man has two neighbors: a man and a woman. And he lives next to a person having a cat.\n4. The Norwegian man lives next to the German and likes cappuccino.\n5. The English woman has two neigbors and her pet is a fish.\n The one with a dog loves espresso.</t>
+  </si>
+  <si>
+    <t>Let's sell the right coffee!</t>
+  </si>
+  <si>
+    <t>Cappuccino</t>
+  </si>
+  <si>
+    <t>Espresso</t>
+  </si>
+  <si>
+    <t>Latte</t>
+  </si>
+  <si>
+    <t>{"0":{"money":0}}</t>
+  </si>
+  <si>
+    <t>Colt told me, "The cashier is sick and you will substitute her. You have to sell the right coffee for each customer. We earn 100 coins per a cup of coffee. You have to earn at least 300 coins. Is it clear?"</t>
+  </si>
+  <si>
+    <t>{"0":{"money":200}}</t>
+  </si>
+  <si>
+    <t>{"0":{"money":100}}</t>
+  </si>
+  <si>
+    <t>{"1":{"money":100}}</t>
+  </si>
+  <si>
+    <t>{"2":{"money":100}}</t>
+  </si>
+  <si>
+    <t>You earned  {self.player['money']} coins.\nWhat will you sell to the first customer?</t>
+  </si>
+  <si>
+    <t>You earned  {self.player['money']} coins.\nWhat will you sell to the second customer?</t>
+  </si>
+  <si>
+    <t>You earned  {self.player['money']} coins.\nWhat will you sell to the third customer?</t>
+  </si>
+  <si>
+    <t>You earned  {self.player['money']} coins.\nWhat will you sell to the forth customer?</t>
+  </si>
+  <si>
+    <t>You totally earned  {self.player['money']} coins.</t>
+  </si>
+  <si>
+    <t>Colt came back and said, "Well done! You worked well and now our organization have some additional money to do what we need to do. Thank you!"</t>
+  </si>
+  <si>
+    <t>Have some rest.</t>
+  </si>
+  <si>
+    <t>Colt came back and said, "You failed. Maybe you can handle it another time."</t>
+  </si>
+  <si>
+    <t>money &gt;= 300 222 223</t>
+  </si>
+  <si>
+    <t>trust_points &gt;= 10 164 162</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1424,6 +1514,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1455,7 +1552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1477,6 +1574,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1759,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L193"/>
+  <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="116" workbookViewId="0">
-      <selection activeCell="L160" sqref="L160"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2654,7 +2754,7 @@
         <v>40</v>
       </c>
       <c r="L45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2769,7 +2869,7 @@
         <v>40</v>
       </c>
       <c r="L50" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -3904,7 +4004,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D112" t="s">
         <v>7</v>
@@ -3972,7 +4072,7 @@
         <v>116</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>289</v>
@@ -4465,16 +4565,16 @@
         <v>142</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D142" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E142" s="7">
         <v>143</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G142" s="7">
         <v>204</v>
@@ -4485,16 +4585,16 @@
         <v>143</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D143" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E143">
         <v>145</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G143">
         <v>144</v>
@@ -4505,10 +4605,10 @@
         <v>144</v>
       </c>
       <c r="B144" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D144" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E144">
         <v>204</v>
@@ -4519,16 +4619,16 @@
         <v>145</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D145" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E145">
         <v>146</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G145">
         <v>150</v>
@@ -4539,16 +4639,16 @@
         <v>146</v>
       </c>
       <c r="B146" s="9" t="s">
+        <v>406</v>
+      </c>
+      <c r="D146" s="9" t="s">
         <v>407</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>408</v>
       </c>
       <c r="E146">
         <v>147</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G146">
         <v>150</v>
@@ -4559,16 +4659,16 @@
         <v>147</v>
       </c>
       <c r="B147" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="D147" s="9" t="s">
         <v>410</v>
-      </c>
-      <c r="D147" s="9" t="s">
-        <v>411</v>
       </c>
       <c r="E147">
         <v>148</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G147">
         <v>150</v>
@@ -4579,22 +4679,22 @@
         <v>148</v>
       </c>
       <c r="B148" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D148" s="9" t="s">
         <v>413</v>
-      </c>
-      <c r="D148" s="9" t="s">
-        <v>414</v>
       </c>
       <c r="E148">
         <v>150</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G148">
         <v>149</v>
       </c>
       <c r="L148" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -4602,10 +4702,10 @@
         <v>149</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D149" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E149">
         <v>144</v>
@@ -4616,16 +4716,16 @@
         <v>150</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D150" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E150" s="2">
         <v>151</v>
       </c>
       <c r="F150" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G150" s="2">
         <v>149</v>
@@ -4636,16 +4736,16 @@
         <v>151</v>
       </c>
       <c r="B151" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="D151" s="9" t="s">
         <v>421</v>
-      </c>
-      <c r="D151" s="9" t="s">
-        <v>422</v>
       </c>
       <c r="E151" s="2">
         <v>152</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G151" s="2">
         <v>202</v>
@@ -4656,22 +4756,22 @@
         <v>152</v>
       </c>
       <c r="B152" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="D152" s="9" t="s">
         <v>424</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>425</v>
       </c>
       <c r="E152" s="2">
         <v>153</v>
       </c>
       <c r="F152" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G152" s="2">
         <v>203</v>
       </c>
       <c r="L152" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="153" spans="1:12">
@@ -4679,16 +4779,16 @@
         <v>153</v>
       </c>
       <c r="B153" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="D153" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="F153" s="9" t="s">
         <v>427</v>
-      </c>
-      <c r="D153" s="12" t="s">
-        <v>451</v>
-      </c>
-      <c r="E153" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F153" s="9" t="s">
-        <v>428</v>
       </c>
       <c r="G153" s="2">
         <v>203</v>
@@ -4699,16 +4799,16 @@
         <v>154</v>
       </c>
       <c r="B154" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="D154" s="9" t="s">
         <v>429</v>
-      </c>
-      <c r="D154" s="9" t="s">
-        <v>430</v>
       </c>
       <c r="E154" s="2">
         <v>155</v>
       </c>
       <c r="F154" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G154">
         <v>156</v>
@@ -4719,10 +4819,10 @@
         <v>155</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D155" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E155" s="2">
         <v>156</v>
@@ -4733,10 +4833,10 @@
         <v>156</v>
       </c>
       <c r="B156" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D156" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E156" s="2">
         <v>157</v>
@@ -4747,10 +4847,10 @@
         <v>157</v>
       </c>
       <c r="B157" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="D157" s="9" t="s">
         <v>434</v>
-      </c>
-      <c r="D157" s="9" t="s">
-        <v>435</v>
       </c>
       <c r="E157" s="2">
         <v>158</v>
@@ -4761,16 +4861,16 @@
         <v>158</v>
       </c>
       <c r="B158" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D158" s="9" t="s">
         <v>436</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>437</v>
       </c>
       <c r="E158" s="2">
         <v>200</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G158">
         <v>201</v>
@@ -4781,16 +4881,16 @@
         <v>200</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E159" s="2">
         <v>144</v>
       </c>
       <c r="L159" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="160" spans="1:12">
@@ -4798,335 +4898,752 @@
         <v>201</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D160" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E160" s="2">
         <v>144</v>
       </c>
       <c r="L160" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12">
       <c r="A161" s="2">
         <v>202</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D161" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E161" s="2">
         <v>144</v>
       </c>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:12">
       <c r="A162" s="2">
         <v>203</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E162" s="2">
         <v>156</v>
       </c>
-    </row>
-    <row r="163" spans="1:5">
+      <c r="L162" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12">
       <c r="A163" s="2">
         <v>204</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5">
+        <v>445</v>
+      </c>
+      <c r="D163" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="E163" s="2">
+        <v>206</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="G163">
+        <v>160</v>
+      </c>
+      <c r="L163" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12">
       <c r="A164" s="2">
         <v>205</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D164" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="E164">
         <v>156</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="165" spans="1:12">
+      <c r="A165" s="2">
+        <v>206</v>
+      </c>
+      <c r="B165" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E165">
+        <v>207</v>
+      </c>
+      <c r="F165" t="s">
+        <v>456</v>
+      </c>
+      <c r="G165">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12">
+      <c r="A166" s="2">
+        <v>207</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="D166" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E166" t="s">
+        <v>461</v>
+      </c>
+      <c r="F166" t="s">
+        <v>456</v>
+      </c>
+      <c r="G166">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12">
+      <c r="A167">
+        <v>208</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="D167" t="s">
+        <v>2</v>
+      </c>
+      <c r="E167">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12">
+      <c r="A168">
+        <v>209</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="D168" t="s">
+        <v>2</v>
+      </c>
+      <c r="E168">
+        <v>211</v>
+      </c>
+      <c r="L168" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12">
+      <c r="A169">
+        <v>210</v>
+      </c>
+      <c r="B169" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="D169" t="s">
+        <v>2</v>
+      </c>
+      <c r="E169">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12">
+      <c r="A170">
+        <v>211</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="D170" t="s">
+        <v>465</v>
+      </c>
+      <c r="E170">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12">
+      <c r="A171">
+        <v>212</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="D171" t="s">
+        <v>466</v>
+      </c>
+      <c r="E171">
+        <v>213</v>
+      </c>
+      <c r="F171" t="s">
+        <v>467</v>
+      </c>
+      <c r="G171">
+        <v>214</v>
+      </c>
+      <c r="H171" t="s">
+        <v>468</v>
+      </c>
+      <c r="I171">
+        <v>214</v>
+      </c>
+      <c r="L171" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12">
+      <c r="A172">
+        <v>213</v>
+      </c>
+      <c r="B172" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="D172" t="s">
+        <v>466</v>
+      </c>
+      <c r="E172">
+        <v>215</v>
+      </c>
+      <c r="F172" t="s">
+        <v>467</v>
+      </c>
+      <c r="G172">
+        <v>216</v>
+      </c>
+      <c r="H172" t="s">
+        <v>468</v>
+      </c>
+      <c r="I172">
+        <v>217</v>
+      </c>
+      <c r="L172" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12">
+      <c r="A173">
+        <v>214</v>
+      </c>
+      <c r="B173" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="D173" t="s">
+        <v>466</v>
+      </c>
+      <c r="E173">
+        <v>215</v>
+      </c>
+      <c r="F173" t="s">
+        <v>467</v>
+      </c>
+      <c r="G173">
+        <v>216</v>
+      </c>
+      <c r="H173" t="s">
+        <v>468</v>
+      </c>
+      <c r="I173">
+        <v>217</v>
+      </c>
+      <c r="L173" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12">
+      <c r="A174">
+        <v>215</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="D174" t="s">
+        <v>466</v>
+      </c>
+      <c r="E174">
+        <v>218</v>
+      </c>
+      <c r="F174" t="s">
+        <v>467</v>
+      </c>
+      <c r="G174">
+        <v>218</v>
+      </c>
+      <c r="H174" t="s">
+        <v>468</v>
+      </c>
+      <c r="I174">
+        <v>219</v>
+      </c>
+      <c r="L174" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12">
+      <c r="A175">
+        <v>216</v>
+      </c>
+      <c r="B175" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="D175" t="s">
+        <v>466</v>
+      </c>
+      <c r="E175">
+        <v>218</v>
+      </c>
+      <c r="F175" t="s">
+        <v>467</v>
+      </c>
+      <c r="G175">
+        <v>218</v>
+      </c>
+      <c r="H175" t="s">
+        <v>468</v>
+      </c>
+      <c r="I175">
+        <v>219</v>
+      </c>
+      <c r="L175" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12">
+      <c r="A176">
+        <v>217</v>
+      </c>
+      <c r="B176" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="D176" t="s">
+        <v>466</v>
+      </c>
+      <c r="E176">
+        <v>218</v>
+      </c>
+      <c r="F176" t="s">
+        <v>467</v>
+      </c>
+      <c r="G176">
+        <v>218</v>
+      </c>
+      <c r="H176" t="s">
+        <v>468</v>
+      </c>
+      <c r="I176">
+        <v>219</v>
+      </c>
+      <c r="L176" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12">
+      <c r="A177">
+        <v>218</v>
+      </c>
+      <c r="B177" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="D177" t="s">
+        <v>466</v>
+      </c>
+      <c r="E177">
+        <v>220</v>
+      </c>
+      <c r="F177" t="s">
+        <v>467</v>
+      </c>
+      <c r="G177">
+        <v>220</v>
+      </c>
+      <c r="H177" t="s">
+        <v>468</v>
+      </c>
+      <c r="I177">
+        <v>221</v>
+      </c>
+      <c r="L177" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12">
+      <c r="A178">
+        <v>219</v>
+      </c>
+      <c r="B178" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="D178" t="s">
+        <v>466</v>
+      </c>
+      <c r="E178">
+        <v>220</v>
+      </c>
+      <c r="F178" t="s">
+        <v>467</v>
+      </c>
+      <c r="G178">
+        <v>220</v>
+      </c>
+      <c r="H178" t="s">
+        <v>468</v>
+      </c>
+      <c r="I178">
+        <v>221</v>
+      </c>
+      <c r="L178" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12">
       <c r="A179">
+        <v>220</v>
+      </c>
+      <c r="B179" t="s">
+        <v>479</v>
+      </c>
+      <c r="D179" t="s">
+        <v>2</v>
+      </c>
+      <c r="E179" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12">
+      <c r="A180">
+        <v>221</v>
+      </c>
+      <c r="B180" t="s">
+        <v>479</v>
+      </c>
+      <c r="D180" t="s">
+        <v>2</v>
+      </c>
+      <c r="E180" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12">
+      <c r="B182" s="9"/>
+    </row>
+    <row r="183" spans="1:12">
+      <c r="B183" s="13"/>
+    </row>
+    <row r="184" spans="1:12">
+      <c r="B184" s="9"/>
+    </row>
+    <row r="189" spans="1:12">
+      <c r="A189">
+        <v>222</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="D189" t="s">
+        <v>481</v>
+      </c>
+      <c r="E189">
         <v>160</v>
       </c>
-      <c r="B179" t="s">
+      <c r="L189" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12">
+      <c r="A190">
+        <v>223</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>482</v>
+      </c>
+      <c r="D190" t="s">
+        <v>481</v>
+      </c>
+      <c r="E190">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12">
+      <c r="A191">
+        <v>160</v>
+      </c>
+      <c r="B191" t="s">
         <v>358</v>
       </c>
-      <c r="D179" t="s">
+      <c r="D191" t="s">
         <v>359</v>
       </c>
-      <c r="E179">
+      <c r="E191">
         <v>161</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
-      <c r="A180">
+    <row r="192" spans="1:12">
+      <c r="A192">
         <v>161</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B192" t="s">
         <v>361</v>
       </c>
-      <c r="D180" s="1" t="s">
+      <c r="D192" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="E180" t="s">
+      <c r="E192" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193">
+        <v>162</v>
+      </c>
+      <c r="B193" t="s">
+        <v>363</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="E193">
+        <v>163</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="G193">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
+      <c r="A194">
+        <v>163</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E194" s="6">
+        <v>169</v>
+      </c>
+      <c r="F194" t="s">
+        <v>368</v>
+      </c>
+      <c r="G194" s="2">
+        <v>169</v>
+      </c>
+      <c r="H194" t="s">
+        <v>369</v>
+      </c>
+      <c r="I194" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
+      <c r="A195">
+        <v>164</v>
+      </c>
+      <c r="B195" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="181" spans="1:11">
-      <c r="A181">
-        <v>162</v>
-      </c>
-      <c r="B181" t="s">
-        <v>363</v>
-      </c>
-      <c r="D181" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="E181">
-        <v>163</v>
-      </c>
-      <c r="F181" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="G181">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="182" spans="1:11">
-      <c r="A182">
-        <v>163</v>
-      </c>
-      <c r="B182" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D182" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="E182" s="6">
+      <c r="D195" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E195">
+        <v>166</v>
+      </c>
+      <c r="F195" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="G195">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11">
+      <c r="A196">
+        <v>165</v>
+      </c>
+      <c r="B196" t="s">
+        <v>373</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E196">
+        <v>166</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="G196" s="2">
         <v>169</v>
       </c>
-      <c r="F182" t="s">
-        <v>368</v>
-      </c>
-      <c r="G182" s="2">
+    </row>
+    <row r="197" spans="1:11">
+      <c r="A197">
+        <v>166</v>
+      </c>
+      <c r="B197" t="s">
+        <v>383</v>
+      </c>
+      <c r="D197" t="s">
+        <v>376</v>
+      </c>
+      <c r="E197" s="2">
+        <v>167</v>
+      </c>
+      <c r="F197" t="s">
+        <v>377</v>
+      </c>
+      <c r="G197" s="2">
+        <v>170</v>
+      </c>
+      <c r="H197" t="s">
+        <v>378</v>
+      </c>
+      <c r="I197" s="2">
+        <v>168</v>
+      </c>
+      <c r="J197" t="s">
+        <v>390</v>
+      </c>
+      <c r="K197">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11">
+      <c r="A198">
+        <v>167</v>
+      </c>
+      <c r="B198" t="s">
+        <v>382</v>
+      </c>
+      <c r="D198" t="s">
+        <v>379</v>
+      </c>
+      <c r="E198" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11">
+      <c r="A199">
+        <v>168</v>
+      </c>
+      <c r="B199" t="s">
+        <v>386</v>
+      </c>
+      <c r="D199" t="s">
+        <v>379</v>
+      </c>
+      <c r="E199" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11">
+      <c r="A200">
         <v>169</v>
       </c>
-      <c r="H182" t="s">
-        <v>369</v>
-      </c>
-      <c r="I182" s="7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11">
-      <c r="A183">
-        <v>164</v>
-      </c>
-      <c r="B183" t="s">
-        <v>371</v>
-      </c>
-      <c r="D183" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="E183">
-        <v>166</v>
-      </c>
-      <c r="F183" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="G183">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="184" spans="1:11">
-      <c r="A184">
-        <v>165</v>
-      </c>
-      <c r="B184" t="s">
-        <v>374</v>
-      </c>
-      <c r="D184" s="1" t="s">
+      <c r="B200" t="s">
+        <v>387</v>
+      </c>
+      <c r="D200" t="s">
+        <v>379</v>
+      </c>
+      <c r="E200" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11">
+      <c r="A201">
+        <v>170</v>
+      </c>
+      <c r="B201" t="s">
+        <v>380</v>
+      </c>
+      <c r="D201" t="s">
+        <v>379</v>
+      </c>
+      <c r="E201" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11">
+      <c r="A202">
+        <v>171</v>
+      </c>
+      <c r="B202" t="s">
+        <v>388</v>
+      </c>
+      <c r="D202" t="s">
+        <v>379</v>
+      </c>
+      <c r="E202" s="2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11">
+      <c r="A203">
+        <v>172</v>
+      </c>
+      <c r="B203" t="s">
+        <v>389</v>
+      </c>
+      <c r="D203" t="s">
         <v>376</v>
       </c>
-      <c r="E184">
-        <v>166</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="G184" s="2">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="185" spans="1:11">
-      <c r="A185">
-        <v>166</v>
-      </c>
-      <c r="B185" t="s">
-        <v>384</v>
-      </c>
-      <c r="D185" t="s">
-        <v>377</v>
-      </c>
-      <c r="E185" s="2">
+      <c r="E203">
         <v>167</v>
       </c>
-      <c r="F185" t="s">
-        <v>378</v>
-      </c>
-      <c r="G185" s="2">
-        <v>170</v>
-      </c>
-      <c r="H185" t="s">
+      <c r="F203" t="s">
+        <v>390</v>
+      </c>
+      <c r="G203">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11">
+      <c r="A204">
+        <v>173</v>
+      </c>
+      <c r="B204" t="s">
+        <v>391</v>
+      </c>
+      <c r="D204" t="s">
         <v>379</v>
       </c>
-      <c r="I185" s="2">
-        <v>168</v>
-      </c>
-      <c r="J185" t="s">
-        <v>391</v>
-      </c>
-      <c r="K185">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="186" spans="1:11">
-      <c r="A186">
-        <v>167</v>
-      </c>
-      <c r="B186" t="s">
-        <v>383</v>
-      </c>
-      <c r="D186" t="s">
-        <v>380</v>
-      </c>
-      <c r="E186" s="2">
+      <c r="E204">
         <v>174</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
-      <c r="A187">
-        <v>168</v>
-      </c>
-      <c r="B187" t="s">
-        <v>387</v>
-      </c>
-      <c r="D187" t="s">
-        <v>380</v>
-      </c>
-      <c r="E187" s="2">
+    <row r="205" spans="1:11">
+      <c r="A205">
         <v>174</v>
       </c>
-    </row>
-    <row r="188" spans="1:11">
-      <c r="A188">
-        <v>169</v>
-      </c>
-      <c r="B188" t="s">
-        <v>388</v>
-      </c>
-      <c r="D188" t="s">
-        <v>380</v>
-      </c>
-      <c r="E188" s="2">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="189" spans="1:11">
-      <c r="A189">
-        <v>170</v>
-      </c>
-      <c r="B189" t="s">
-        <v>381</v>
-      </c>
-      <c r="D189" t="s">
-        <v>380</v>
-      </c>
-      <c r="E189" s="2">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="190" spans="1:11">
-      <c r="A190">
-        <v>171</v>
-      </c>
-      <c r="B190" t="s">
-        <v>389</v>
-      </c>
-      <c r="D190" t="s">
-        <v>380</v>
-      </c>
-      <c r="E190" s="2">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="191" spans="1:11">
-      <c r="A191">
-        <v>172</v>
-      </c>
-      <c r="B191" t="s">
-        <v>390</v>
-      </c>
-      <c r="D191" t="s">
-        <v>377</v>
-      </c>
-      <c r="E191">
-        <v>167</v>
-      </c>
-      <c r="F191" t="s">
-        <v>391</v>
-      </c>
-      <c r="G191">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="192" spans="1:11">
-      <c r="A192">
-        <v>173</v>
-      </c>
-      <c r="B192" t="s">
+      <c r="B205" t="s">
         <v>392</v>
       </c>
-      <c r="D192" t="s">
-        <v>380</v>
-      </c>
-      <c r="E192">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7">
-      <c r="A193">
-        <v>174</v>
-      </c>
-      <c r="B193" t="s">
+      <c r="D205" t="s">
         <v>393</v>
       </c>
-      <c r="D193" t="s">
+      <c r="E205">
+        <v>1</v>
+      </c>
+      <c r="F205" t="s">
         <v>394</v>
       </c>
-      <c r="E193">
-        <v>1</v>
-      </c>
-      <c r="F193" t="s">
-        <v>395</v>
-      </c>
-      <c r="G193">
+      <c r="G205">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix the bug in script line 49
</commit_message>
<xml_diff>
--- a/Template.xlsx
+++ b/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kirillsafonov/PycharmProjects/blade_runner_bot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D81E9C-B012-2C42-8C43-B66408A5CFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6925FC6D-128F-8749-8A44-3448D549B757}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1482,7 +1482,7 @@
     <t>trust_points &gt;= 10 164 162</t>
   </si>
   <si>
-    <t>{"0":{"photo_flag":1}]</t>
+    <t>{"0":{"photo_flag":1}}</t>
   </si>
 </sst>
 </file>
@@ -1859,8 +1859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A183" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G192" sqref="G192"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O54" sqref="N54:O54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>